<commit_message>
New changes to graphs
- Added age stratification for smoking and alcohol usage in England
- Added new source of data for fertility rates and plotted them
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/Position Paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{C948A297-A85F-4657-A8D7-496A4B9E4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB46F25-5925-4020-B9BE-C36A4E4322D5}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{C948A297-A85F-4657-A8D7-496A4B9E4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{233B4BC3-A642-4820-8000-C2CE0C206E31}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="5985" windowWidth="19440" windowHeight="15000" xr2:uid="{12692E29-F9EF-4526-8740-C69123C14B2D}"/>
+    <workbookView xWindow="28635" yWindow="-165" windowWidth="24330" windowHeight="13230" xr2:uid="{12692E29-F9EF-4526-8740-C69123C14B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="106">
   <si>
     <t>BMI</t>
   </si>
@@ -2004,6 +2004,16 @@
 Age groups: [16-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75+, All adults]
 Groups: [Male, Female, All adults]</t>
     </r>
+  </si>
+  <si>
+    <t>Births in England and Wales</t>
+  </si>
+  <si>
+    <t>Fertility Rates
+Cats: NA
+Years: [1938-2022]
+Age groups: [&gt;20, 20-24, 25-29, 30-34, 35-39, 40-44, 45&lt;]
+Groups: NA</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2236,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2334,6 +2344,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2655,23 +2668,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA4EAD-0BC0-4667-A29D-D85C3908A55B}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="5"/>
+    <col min="3" max="3" width="41.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="41.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.7265625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -2697,7 +2710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="33" t="s">
         <v>70</v>
       </c>
@@ -2723,7 +2736,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="34"/>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -2741,7 +2754,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="34"/>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -2762,7 +2775,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="28" customFormat="1" ht="256.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="28" customFormat="1" ht="247.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="35"/>
       <c r="B5" s="23" t="s">
         <v>15</v>
@@ -2782,7 +2795,7 @@
       <c r="G5" s="26"/>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="37" t="s">
         <v>84</v>
       </c>
@@ -2796,7 +2809,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="34"/>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -2808,7 +2821,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="34"/>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -2820,7 +2833,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="35"/>
       <c r="B9" s="23" t="s">
         <v>15</v>
@@ -2836,7 +2849,7 @@
       <c r="G9" s="26"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="36" t="s">
         <v>0</v>
       </c>
@@ -2856,7 +2869,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="256.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="247.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="36"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
@@ -2874,7 +2887,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="36"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -2892,7 +2905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="36"/>
       <c r="B13" s="23" t="s">
         <v>15</v>
@@ -2912,7 +2925,7 @@
       <c r="G13" s="26"/>
       <c r="H13" s="27"/>
     </row>
-    <row r="14" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="36" t="s">
         <v>1</v>
       </c>
@@ -2926,7 +2939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="36"/>
       <c r="B15" s="2" t="s">
         <v>11</v>
@@ -2938,7 +2951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>12</v>
@@ -2950,7 +2963,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="28" customFormat="1" ht="346.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="28" customFormat="1" ht="334.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="36"/>
       <c r="B17" s="23" t="s">
         <v>15</v>
@@ -2966,7 +2979,7 @@
       <c r="G17" s="26"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="36" t="s">
         <v>2</v>
       </c>
@@ -2980,7 +2993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="36"/>
       <c r="B19" s="2" t="s">
         <v>11</v>
@@ -2992,7 +3005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
@@ -3004,7 +3017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="36"/>
       <c r="B21" s="23" t="s">
         <v>15</v>
@@ -3020,7 +3033,7 @@
       <c r="G21" s="26"/>
       <c r="H21" s="27"/>
     </row>
-    <row r="22" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="36" t="s">
         <v>3</v>
       </c>
@@ -3034,7 +3047,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="36"/>
       <c r="B23" s="2" t="s">
         <v>11</v>
@@ -3046,7 +3059,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="36"/>
       <c r="B24" s="2" t="s">
         <v>12</v>
@@ -3058,7 +3071,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="36"/>
       <c r="B25" s="23" t="s">
         <v>15</v>
@@ -3074,7 +3087,7 @@
       <c r="G25" s="26"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="36" t="s">
         <v>4</v>
       </c>
@@ -3093,8 +3106,14 @@
       <c r="F26" s="20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="36"/>
       <c r="B27" s="2" t="s">
         <v>11</v>
@@ -3106,7 +3125,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="36"/>
       <c r="B28" s="2" t="s">
         <v>12</v>
@@ -3123,8 +3142,14 @@
       <c r="F28" s="20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="36"/>
       <c r="B29" s="23" t="s">
         <v>15</v>
@@ -3140,7 +3165,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="27"/>
     </row>
-    <row r="30" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="36" t="s">
         <v>8</v>
       </c>
@@ -3160,7 +3185,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="36"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
@@ -3178,7 +3203,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="36"/>
       <c r="B32" s="2" t="s">
         <v>12</v>
@@ -3196,7 +3221,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="36"/>
       <c r="B33" s="23" t="s">
         <v>15</v>
@@ -3216,7 +3241,7 @@
       <c r="G33" s="26"/>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="36" t="s">
         <v>5</v>
       </c>
@@ -3236,7 +3261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="36"/>
       <c r="B35" s="2" t="s">
         <v>11</v>
@@ -3251,7 +3276,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="36"/>
       <c r="B36" s="2" t="s">
         <v>12</v>
@@ -3266,7 +3291,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="36"/>
       <c r="B37" s="23" t="s">
         <v>15</v>
@@ -3284,7 +3309,7 @@
       <c r="G37" s="26"/>
       <c r="H37" s="27"/>
     </row>
-    <row r="38" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="36" t="s">
         <v>6</v>
       </c>
@@ -3301,7 +3326,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="36"/>
       <c r="B39" s="2" t="s">
         <v>11</v>
@@ -3316,7 +3341,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="36"/>
       <c r="B40" s="2" t="s">
         <v>12</v>
@@ -3331,7 +3356,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="36"/>
       <c r="B41" s="23" t="s">
         <v>15</v>
@@ -3349,7 +3374,7 @@
       <c r="G41" s="26"/>
       <c r="H41" s="27"/>
     </row>
-    <row r="42" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="36" t="s">
         <v>7</v>
       </c>
@@ -3375,7 +3400,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="36"/>
       <c r="B43" s="2" t="s">
         <v>11</v>
@@ -3391,7 +3416,7 @@
       </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="36"/>
       <c r="B44" s="2" t="s">
         <v>12</v>
@@ -3404,7 +3429,7 @@
       </c>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:8" s="28" customFormat="1" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" s="28" customFormat="1" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="36"/>
       <c r="B45" s="23" t="s">
         <v>15</v>
@@ -3420,7 +3445,7 @@
       <c r="G45" s="26"/>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="160.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="36" t="s">
         <v>9</v>
       </c>
@@ -3434,7 +3459,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="36"/>
       <c r="B47" s="2" t="s">
         <v>11</v>
@@ -3446,7 +3471,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="36"/>
       <c r="B48" s="2" t="s">
         <v>12</v>
@@ -3458,7 +3483,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" s="28" customFormat="1" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="36"/>
       <c r="B49" s="23" t="s">
         <v>15</v>
@@ -3474,7 +3499,7 @@
       <c r="G49" s="26"/>
       <c r="H49" s="27"/>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A2:A5"/>
@@ -3556,9 +3581,11 @@
     <hyperlink ref="E5" r:id="rId63" xr:uid="{1BC3BC20-D480-460C-B729-36775E453454}"/>
     <hyperlink ref="G2" r:id="rId64" xr:uid="{176DF67B-3596-4BD3-AEEE-8611ECE9A3F8}"/>
     <hyperlink ref="G4" r:id="rId65" xr:uid="{F24B6F9D-DDCA-459E-810C-D3F28388B853}"/>
+    <hyperlink ref="G26" r:id="rId66" xr:uid="{A7444995-440A-42F1-9C16-6C33A43AB8F8}"/>
+    <hyperlink ref="G28" r:id="rId67" xr:uid="{E3020E44-D17C-4F27-821A-57C4580FB907}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
 
@@ -3570,32 +3597,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="102.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Changes and additions to plots
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{C948A297-A85F-4657-A8D7-496A4B9E4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5372AA6-FA5B-4CDE-8561-94212794624F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{12692E29-F9EF-4526-8740-C69123C14B2D}"/>
+    <workbookView xWindow="-38520" yWindow="105" windowWidth="38640" windowHeight="21240" xr2:uid="{12692E29-F9EF-4526-8740-C69123C14B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="2" r:id="rId1"/>
@@ -2668,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA4EAD-0BC0-4667-A29D-D85C3908A55B}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding plots for diet
</commit_message>
<xml_diff>
--- a/Data Sources.xlsx
+++ b/Data Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/UK-cancer-trends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{C948A297-A85F-4657-A8D7-496A4B9E4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5372AA6-FA5B-4CDE-8561-94212794624F}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="13_ncr:1_{C948A297-A85F-4657-A8D7-496A4B9E4341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B830BE90-1C1D-4BA3-AF8F-9D7C817E720E}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="105" windowWidth="38640" windowHeight="21240" xr2:uid="{12692E29-F9EF-4526-8740-C69123C14B2D}"/>
   </bookViews>
@@ -2236,11 +2236,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2264,15 +2261,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2314,9 +2302,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2329,9 +2314,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2668,842 +2650,842 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDA4EAD-0BC0-4667-A29D-D85C3908A55B}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="101.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="41.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="101.42578125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.7109375" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="28" customFormat="1" ht="256.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="1:8" s="23" customFormat="1" ht="256.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+      <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30"/>
+      <c r="B9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="256.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="13" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31"/>
+      <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="28" customFormat="1" ht="346.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="23" t="s">
+    <row r="17" spans="1:8" s="23" customFormat="1" ht="346.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="31"/>
+      <c r="B17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="31"/>
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="31"/>
+      <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="37"/>
-      <c r="B21" s="23" t="s">
+    <row r="21" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="31"/>
+      <c r="B21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="31"/>
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="23" t="s">
+    <row r="25" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31"/>
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="26"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="16" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
-      <c r="B27" s="2" t="s">
+      <c r="A27" s="31"/>
+      <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H28" s="33" t="s">
+      <c r="H28" s="16" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="37"/>
-      <c r="B29" s="23" t="s">
+    <row r="29" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31"/>
+      <c r="B29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="27"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
-      <c r="B31" s="2" t="s">
+      <c r="A31" s="31"/>
+      <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="16" t="s">
+      <c r="F31" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
-      <c r="B33" s="23" t="s">
+    <row r="33" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="31"/>
+      <c r="B33" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="26"/>
     </row>
     <row r="34" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
-      <c r="B36" s="2" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
-      <c r="B37" s="23" t="s">
+    <row r="37" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
+      <c r="B37" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="27"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37"/>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="31"/>
+      <c r="B40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37"/>
-      <c r="B41" s="23" t="s">
+    <row r="41" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="31"/>
+      <c r="B41" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="31"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="27"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="37"/>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E43" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H43" s="1"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:8" s="28" customFormat="1" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
-      <c r="B45" s="23" t="s">
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" s="23" customFormat="1" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="31"/>
+      <c r="B45" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="25" t="s">
+      <c r="D45" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="26"/>
     </row>
     <row r="46" spans="1:8" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="17" t="s">
+      <c r="D46" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="2" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D47" s="17" t="s">
+      <c r="D47" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37"/>
-      <c r="B48" s="2" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="28" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="37"/>
-      <c r="B49" s="23" t="s">
+    <row r="49" spans="1:8" s="23" customFormat="1" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="31"/>
+      <c r="B49" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="27"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="26"/>
     </row>
     <row r="50" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3625,7 +3607,7 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="9" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>